<commit_message>
added the ready templates for displaying chart and exporting values
</commit_message>
<xml_diff>
--- a/exports/Reports.xlsx
+++ b/exports/Reports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Pyetja</t>
   </si>
@@ -25,37 +25,16 @@
     <t>Totali</t>
   </si>
   <si>
-    <t>Cilat dokumente/informata janë publike në faqen tuaj të internetit?</t>
-  </si>
-  <si>
-    <t>Aktivitetet kryesore</t>
-  </si>
-  <si>
-    <t>Anëtarët e Kuvendit/Bordit</t>
-  </si>
-  <si>
-    <t>Dokumentet e brendshme</t>
-  </si>
-  <si>
-    <t>Donatorët</t>
-  </si>
-  <si>
-    <t>Emrat e stafit</t>
-  </si>
-  <si>
-    <t>Fushat e punës</t>
-  </si>
-  <si>
-    <t>Misioni i organizatës</t>
-  </si>
-  <si>
-    <t>Projektet</t>
-  </si>
-  <si>
-    <t>Raportet Financiare</t>
-  </si>
-  <si>
-    <t>Raportet Narrative</t>
+    <t>Si do ta vlerësonit përzgjedhjen e çështjeve për t’u trajtuar nga organizatat e shoqërisë civile në kuadër të aktiviteteve të tyre?</t>
+  </si>
+  <si>
+    <t>Të bazuara në analizën e brengave të grupeve që i përfaqësojnë</t>
+  </si>
+  <si>
+    <t>Të bazuara në fondet në dispozicion</t>
+  </si>
+  <si>
+    <t>Të bazuara në kontaktet e drejtpërdrejta me grupet që i përfaqësojnë</t>
   </si>
 </sst>
 </file>
@@ -410,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,7 +417,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -446,7 +425,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="4">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -454,63 +433,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>